<commit_message>
Update Tabella tempi ed errori partecipanti.xlsx
</commit_message>
<xml_diff>
--- a/Tabella tempi ed errori partecipanti.xlsx
+++ b/Tabella tempi ed errori partecipanti.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dw/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dw/Desktop/DSML/ProgettoDSML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50898C85-7445-4046-8512-6EBB10627699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166F1156-2088-EC4A-BB05-2CD60A82E555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" xr2:uid="{A695641D-8FD7-0041-92E1-74436705CA24}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +121,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -159,30 +166,17 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -193,19 +187,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD12403-B5CE-0447-A6E1-57A965DA9321}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,296 +596,1110 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5">
+      <c r="A2" s="5">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
         <f>B2+D2+F2+H2+J2</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
+        <v>15</v>
+      </c>
+      <c r="M2" s="6">
         <f>C2+E2+G2+I2+K2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="7">
+      <c r="A3" s="5">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>25</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
         <f>B3+D3+F3+H3+J3</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="7">
+        <v>30</v>
+      </c>
+      <c r="M3" s="6">
         <f>C3+E3+G3+I3+K3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="7">
-        <f t="shared" ref="L4:L15" si="0">B4+D4+F4+H4+J4</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="7">
-        <f t="shared" ref="M4:M15" si="1">C4+E4+G4+I4+K4</f>
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>40</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <f t="shared" ref="L4:L17" si="0">B4+D4+F4+H4+J4</f>
+        <v>42</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" ref="M4:M17" si="1">C4+E4+G4+I4+K4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="7">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="7">
+        <v>15</v>
+      </c>
+      <c r="M5" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="7">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>10</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
+        <v>13</v>
+      </c>
+      <c r="M6" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="7">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>60</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
+        <v>62</v>
+      </c>
+      <c r="M7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="7">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>125</v>
+      </c>
+      <c r="G8" s="5">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
+        <v>136</v>
+      </c>
+      <c r="M8" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="7">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="7">
+        <v>53</v>
+      </c>
+      <c r="M9" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="7">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>2</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2</v>
+      </c>
+      <c r="J10" s="7">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="7">
+        <v>5</v>
+      </c>
+      <c r="M10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="7">
+      <c r="A11" s="5">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>78</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="7">
+        <v>83</v>
+      </c>
+      <c r="M11" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="7">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>87</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="7">
+        <v>94</v>
+      </c>
+      <c r="M12" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="7">
+      <c r="A13" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>146</v>
+      </c>
+      <c r="G13" s="2">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="7">
+        <v>148</v>
+      </c>
+      <c r="M13" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="A14" s="5">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
       <c r="L14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="7">
+        <v>10</v>
+      </c>
+      <c r="M14" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="7">
+      <c r="A15" s="5">
+        <v>6</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>30</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="7">
+        <v>40</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>60</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="M16" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>103</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>7</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>10</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>10</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>1</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" ref="L18:L21" si="2">B18+D18+F18+H18+J18</f>
+        <v>22</v>
+      </c>
+      <c r="M18" s="8">
+        <f t="shared" ref="M18:M21" si="3">C18+E18+G18+I18+K18</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>4</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>60</v>
+      </c>
+      <c r="G19" s="5">
+        <v>4</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="M19" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>7</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>120</v>
+      </c>
+      <c r="G20" s="5">
+        <v>2</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="M20" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>106</v>
+      </c>
+      <c r="G21" s="2">
+        <v>4</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>8</v>
+      </c>
+      <c r="B22" s="9">
+        <v>60</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>4</v>
+      </c>
+      <c r="I22" s="9">
+        <v>1</v>
+      </c>
+      <c r="J22" s="9">
+        <v>1</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="10">
+        <v>0</v>
+      </c>
+      <c r="M22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>8</v>
+      </c>
+      <c r="B23" s="9">
+        <v>2</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>4</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>40</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0</v>
+      </c>
+      <c r="M23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>8</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>3</v>
+      </c>
+      <c r="G24" s="9">
+        <v>1</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0</v>
+      </c>
+      <c r="L24" s="10">
+        <v>0</v>
+      </c>
+      <c r="M24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="12">
+        <v>8</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <v>6</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>165</v>
+      </c>
+      <c r="G25" s="12">
+        <v>4</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
+        <v>0</v>
+      </c>
+      <c r="M25" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>9</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="10">
+        <v>0</v>
+      </c>
+      <c r="M26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>9</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="10">
+        <v>0</v>
+      </c>
+      <c r="M27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>9</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="10">
+        <v>0</v>
+      </c>
+      <c r="M28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="12">
+        <v>9</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="13">
+        <v>0</v>
+      </c>
+      <c r="M29" s="13">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiornamento excel ed inizio capitolo studio usabilità
</commit_message>
<xml_diff>
--- a/Tabella tempi ed errori partecipanti.xlsx
+++ b/Tabella tempi ed errori partecipanti.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dw/Desktop/DSML/ProgettoDSML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBCDEC0-98B4-6341-8007-0D4D9FBEC127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EB9D6D-42DE-4147-80F0-110D021D8ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" xr2:uid="{A695641D-8FD7-0041-92E1-74436705CA24}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Numero partecipante</t>
   </si>
@@ -100,6 +100,10 @@
   <si>
     <t>Errori annulla 
 operatore</t>
+  </si>
+  <si>
+    <t>Errori individuazione
+ configurazione</t>
   </si>
 </sst>
 </file>
@@ -534,7 +538,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -944,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -956,30 +960,30 @@
         <v>0</v>
       </c>
       <c r="F10" s="7">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="G10" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H10" s="7">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="I10" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="7">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="K10" s="7">
         <v>0</v>
       </c>
       <c r="L10" s="8">
         <f t="shared" ref="L10:L13" si="4">B10+D10+F10+H10+J10</f>
-        <v>175</v>
+        <v>47</v>
       </c>
       <c r="M10" s="8">
         <f t="shared" ref="M10:M13" si="5">C10+E10+G10+I10+K10</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -987,10 +991,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="5">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -999,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G11" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5">
         <v>0</v>
@@ -1018,57 +1022,97 @@
       </c>
       <c r="L11" s="6">
         <f t="shared" si="4"/>
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="B12" s="5">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>250</v>
+      </c>
+      <c r="G12" s="5">
+        <v>3</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
       <c r="L12" s="6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>258</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>120</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
       <c r="L13" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="M13" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finito forse il documento
</commit_message>
<xml_diff>
--- a/Tabella tempi ed errori partecipanti.xlsx
+++ b/Tabella tempi ed errori partecipanti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dw/Desktop/DSML/ProgettoDSML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EB9D6D-42DE-4147-80F0-110D021D8ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588F5A5E-EDFD-9E4E-A424-064CDDFAB1A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" xr2:uid="{A695641D-8FD7-0041-92E1-74436705CA24}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Numero partecipante</t>
   </si>
@@ -104,6 +104,21 @@
   <si>
     <t>Errori individuazione
  configurazione</t>
+  </si>
+  <si>
+    <t>Tempo di esecuzione</t>
+  </si>
+  <si>
+    <t>Errori</t>
+  </si>
+  <si>
+    <t>Errori icone</t>
+  </si>
+  <si>
+    <t>Errori task</t>
+  </si>
+  <si>
+    <t>Tempo task</t>
   </si>
 </sst>
 </file>
@@ -180,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -209,16 +224,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -227,6 +236,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7F0000"/>
+      <color rgb="FFB20000"/>
+      <color rgb="FFDA0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -236,6 +252,3353 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tempo d'azione complessivo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tempo di esecuzione</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Foglio1!$N$6,Foglio1!$N$10,Foglio1!$N$14,Foglio1!$N$18,Foglio1!$N$22,Foglio1!$N$26,Foglio1!$N$30,Foglio1!$N$34,Foglio1!$N$38,Foglio1!$N$42)</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>543</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E5A-7F42-A302-90E092EEE07F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="269845936"/>
+        <c:axId val="269638688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="269845936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Candidato</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269638688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="269638688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Tempo (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269845936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Errori complessivi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Errori icone</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7F0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Foglio1!$P$6,Foglio1!$P$10,Foglio1!$P$14,Foglio1!$P$18,Foglio1!$P$22,Foglio1!$P$26,Foglio1!$P$30,Foglio1!$P$34,Foglio1!$P$38,Foglio1!$P$42)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6CE5-7B40-803A-78082257F5B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Errori task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DA0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Foglio1!$Q$6,Foglio1!$Q$10,Foglio1!$Q$14,Foglio1!$Q$18,Foglio1!$Q$22,Foglio1!$Q$26,Foglio1!$Q$30,Foglio1!$Q$34,Foglio1!$Q$38,Foglio1!$Q$42)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6CE5-7B40-803A-78082257F5B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="271619840"/>
+        <c:axId val="272034752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="271619840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Candidato</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="272034752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="272034752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Numero</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> errori</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="271619840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Tempo d'azione complessivo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Task 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Foglio1!$L$6,Foglio1!$L$10,Foglio1!$L$14,Foglio1!$L$18,Foglio1!$L$22,Foglio1!$L$26,Foglio1!$L$30,Foglio1!$L$34,Foglio1!$L$38,Foglio1!$L$42)</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-69B9-3C4A-A5CF-FE0F94DEE756}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Task 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Foglio1!$L$7,Foglio1!$L$11,Foglio1!$L$15,Foglio1!$L$19,Foglio1!$L$23,Foglio1!$L$27,Foglio1!$L$31,Foglio1!$L$35,Foglio1!$L$39,Foglio1!$L$43)</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-69B9-3C4A-A5CF-FE0F94DEE756}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Task 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Foglio1!$L$8,Foglio1!$L$12,Foglio1!$L$16,Foglio1!$L$20,Foglio1!$L$24,Foglio1!$L$28,Foglio1!$L$32,Foglio1!$L$36,Foglio1!$L$40,Foglio1!$L$44)</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-69B9-3C4A-A5CF-FE0F94DEE756}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Task 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Foglio1!$L$9,Foglio1!$L$13,Foglio1!$L$17,Foglio1!$L$21,Foglio1!$L$25,Foglio1!$L$29,Foglio1!$L$33,Foglio1!$L$37,Foglio1!$L$41,Foglio1!$L$45)</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>189</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-69B9-3C4A-A5CF-FE0F94DEE756}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="270836800"/>
+        <c:axId val="270838432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="270836800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Candidato</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="270838432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="270838432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Tempo (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="270836800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>224370</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8381A7EB-6844-794C-BA96-A1135F4C7CDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>8890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>607910</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>59690</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Grafico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61EFA4DF-0EDC-E745-8C7F-7D09CCC13113}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>421640</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>5080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Grafico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A87360D9-0F08-5E4D-8D61-A31831790664}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,10 +3898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD12403-B5CE-0447-A6E1-57A965DA9321}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,7 +3921,7 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -598,8 +3961,23 @@
       <c r="M1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -641,8 +4019,24 @@
         <f t="shared" ref="M2:M5" si="1">C2+E2+G2+I2+K2</f>
         <v>5</v>
       </c>
+      <c r="N2" s="11">
+        <f>SUM(L2:L5)</f>
+        <v>149</v>
+      </c>
+      <c r="O2" s="11">
+        <f>P2+Q2</f>
+        <v>8</v>
+      </c>
+      <c r="P2" s="1">
+        <f>SUM(I2:I5)+SUM(K2:K5)</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>SUM(C2:C5)+SUM(E2:E5)+SUM(G2:G5)</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -684,8 +4078,9 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -727,8 +4122,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -770,8 +4166,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -813,8 +4210,24 @@
         <f t="shared" ref="M6:M9" si="3">C6+E6+G6+I6+K6</f>
         <v>6</v>
       </c>
+      <c r="N6" s="11">
+        <f>SUM(L6:L9)</f>
+        <v>252</v>
+      </c>
+      <c r="O6" s="11">
+        <f>P6+Q6</f>
+        <v>13</v>
+      </c>
+      <c r="P6" s="1">
+        <f>SUM(I6:I9)+SUM(K6:K9)</f>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>SUM(C6:C9)+SUM(E6:E9)+SUM(G6:G9)</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -857,7 +4270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -900,7 +4313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -943,7 +4356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -985,8 +4398,24 @@
         <f t="shared" ref="M10:M13" si="5">C10+E10+G10+I10+K10</f>
         <v>1</v>
       </c>
+      <c r="N10" s="11">
+        <f>SUM(L10:L13)</f>
+        <v>543</v>
+      </c>
+      <c r="O10" s="11">
+        <f>P10+Q10</f>
+        <v>6</v>
+      </c>
+      <c r="P10" s="1">
+        <f>SUM(I10:I13)+SUM(K10:K13)</f>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>SUM(C10:C13)+SUM(E10:E13)+SUM(G10:G13)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -1029,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -1072,7 +4501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -1115,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>3</v>
       </c>
@@ -1157,8 +4586,24 @@
         <f>C14+E14+G14+I14+K14</f>
         <v>1</v>
       </c>
+      <c r="N14" s="11">
+        <f>SUM(L14:L17)</f>
+        <v>102</v>
+      </c>
+      <c r="O14" s="11">
+        <f>P14+Q14</f>
+        <v>1</v>
+      </c>
+      <c r="P14" s="1">
+        <f>SUM(I14:I17)+SUM(K14:K17)</f>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>SUM(C14:C17)+SUM(E14:E17)+SUM(G14:G17)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>3</v>
       </c>
@@ -1201,7 +4646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -1244,7 +4689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -1287,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>4</v>
       </c>
@@ -1329,8 +4774,24 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
+      <c r="N18" s="11">
+        <f>SUM(L18:L21)</f>
+        <v>264</v>
+      </c>
+      <c r="O18" s="11">
+        <f>P18+Q18</f>
+        <v>6</v>
+      </c>
+      <c r="P18" s="1">
+        <f>SUM(I18:I21)+SUM(K18:K21)</f>
+        <v>1</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>SUM(C18:C21)+SUM(E18:E21)+SUM(G18:G21)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>4</v>
       </c>
@@ -1373,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>4</v>
       </c>
@@ -1416,7 +4877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -1459,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>5</v>
       </c>
@@ -1501,8 +4962,24 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="N22" s="11">
+        <f>SUM(L22:L25)</f>
+        <v>330</v>
+      </c>
+      <c r="O22" s="11">
+        <f>P22+Q22</f>
+        <v>19</v>
+      </c>
+      <c r="P22" s="1">
+        <f>SUM(I22:I25)+SUM(K22:K25)</f>
+        <v>2</v>
+      </c>
+      <c r="Q22" s="1">
+        <f>SUM(C22:C25)+SUM(E22:E25)+SUM(G22:G25)</f>
+        <v>17</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>5</v>
       </c>
@@ -1545,7 +5022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>5</v>
       </c>
@@ -1588,7 +5065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>5</v>
       </c>
@@ -1631,7 +5108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>6</v>
       </c>
@@ -1673,8 +5150,24 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
+      <c r="N26" s="11">
+        <f>SUM(L26:L29)</f>
+        <v>224</v>
+      </c>
+      <c r="O26" s="11">
+        <f>P26+Q26</f>
+        <v>8</v>
+      </c>
+      <c r="P26" s="1">
+        <f>SUM(I26:I29)+SUM(K26:K29)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
+        <f>SUM(C26:C29)+SUM(E26:E29)+SUM(G26:G29)</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>6</v>
       </c>
@@ -1717,7 +5210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>6</v>
       </c>
@@ -1760,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>6</v>
       </c>
@@ -1803,7 +5296,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>7</v>
       </c>
@@ -1838,15 +5331,31 @@
         <v>0</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" ref="L30:L33" si="8">B30+D30+F30+H30+J30</f>
+        <f t="shared" ref="L30:L45" si="8">B30+D30+F30+H30+J30</f>
         <v>22</v>
       </c>
       <c r="M30" s="8">
-        <f t="shared" ref="M30:M33" si="9">C30+E30+G30+I30+K30</f>
+        <f t="shared" ref="M30:M45" si="9">C30+E30+G30+I30+K30</f>
         <v>3</v>
       </c>
+      <c r="N30" s="11">
+        <f>SUM(L30:L33)</f>
+        <v>328</v>
+      </c>
+      <c r="O30" s="11">
+        <f>P30+Q30</f>
+        <v>13</v>
+      </c>
+      <c r="P30" s="1">
+        <f>SUM(I30:I33)+SUM(K30:K33)</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
+        <f>SUM(C30:C33)+SUM(E30:E33)+SUM(G30:G33)</f>
+        <v>13</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>7</v>
       </c>
@@ -1889,7 +5398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>7</v>
       </c>
@@ -1932,7 +5441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>7</v>
       </c>
@@ -1975,7 +5484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>8</v>
       </c>
@@ -2009,14 +5518,32 @@
       <c r="K34" s="9">
         <v>0</v>
       </c>
-      <c r="L34" s="10">
-        <v>0</v>
-      </c>
-      <c r="M34" s="11">
-        <v>0</v>
+      <c r="L34" s="6">
+        <f t="shared" si="8"/>
+        <v>66</v>
+      </c>
+      <c r="M34" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="N34" s="11">
+        <f>SUM(L34:L37)</f>
+        <v>290</v>
+      </c>
+      <c r="O34" s="11">
+        <f>P34+Q34</f>
+        <v>8</v>
+      </c>
+      <c r="P34" s="1">
+        <f>SUM(I34:I37)+SUM(K34:K37)</f>
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1">
+        <f>SUM(C34:C37)+SUM(E34:E37)+SUM(G34:G37)</f>
+        <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>8</v>
       </c>
@@ -2050,14 +5577,16 @@
       <c r="K35" s="9">
         <v>0</v>
       </c>
-      <c r="L35" s="10">
-        <v>0</v>
-      </c>
-      <c r="M35" s="10">
-        <v>0</v>
+      <c r="L35" s="6">
+        <f t="shared" si="8"/>
+        <v>46</v>
+      </c>
+      <c r="M35" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>8</v>
       </c>
@@ -2091,140 +5620,440 @@
       <c r="K36" s="9">
         <v>0</v>
       </c>
-      <c r="L36" s="10">
-        <v>0</v>
-      </c>
-      <c r="M36" s="10">
-        <v>0</v>
+      <c r="L36" s="6">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="M36" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="12">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="10">
         <v>8</v>
       </c>
-      <c r="B37" s="12">
-        <v>1</v>
-      </c>
-      <c r="C37" s="12">
-        <v>0</v>
-      </c>
-      <c r="D37" s="12">
+      <c r="B37" s="10">
+        <v>1</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
         <v>6</v>
       </c>
-      <c r="E37" s="12">
-        <v>0</v>
-      </c>
-      <c r="F37" s="12">
+      <c r="E37" s="10">
+        <v>0</v>
+      </c>
+      <c r="F37" s="10">
         <v>165</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="10">
         <v>4</v>
       </c>
-      <c r="H37" s="12">
-        <v>0</v>
-      </c>
-      <c r="I37" s="12">
-        <v>0</v>
-      </c>
-      <c r="J37" s="12">
-        <v>0</v>
-      </c>
-      <c r="K37" s="12">
-        <v>0</v>
-      </c>
-      <c r="L37" s="13">
-        <v>0</v>
-      </c>
-      <c r="M37" s="13">
-        <v>0</v>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0</v>
+      </c>
+      <c r="K37" s="10">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4">
+        <f t="shared" si="8"/>
+        <v>172</v>
+      </c>
+      <c r="M37" s="4">
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
         <v>9</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="10">
-        <v>0</v>
-      </c>
-      <c r="M38" s="11">
-        <v>0</v>
+      <c r="B38" s="9">
+        <v>10</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <v>4</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0</v>
+      </c>
+      <c r="G38" s="9">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9">
+        <v>5</v>
+      </c>
+      <c r="I38" s="9">
+        <v>1</v>
+      </c>
+      <c r="J38" s="9">
+        <v>2</v>
+      </c>
+      <c r="K38" s="9">
+        <v>0</v>
+      </c>
+      <c r="L38" s="6">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+      <c r="M38" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="N38" s="11">
+        <f>SUM(L38:L41)</f>
+        <v>283</v>
+      </c>
+      <c r="O38" s="11">
+        <f>SUM(M38:M41)</f>
+        <v>7</v>
+      </c>
+      <c r="P38" s="1">
+        <f>SUM(I38:I41)+SUM(K38:K41)</f>
+        <v>1</v>
+      </c>
+      <c r="Q38" s="1">
+        <f>SUM(C38:C41)+SUM(E38:E41)+SUM(G38:G41)</f>
+        <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>9</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="10">
-        <v>0</v>
-      </c>
-      <c r="M39" s="10">
-        <v>0</v>
+      <c r="B39" s="9">
+        <v>4</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+      <c r="D39" s="9">
+        <v>3</v>
+      </c>
+      <c r="E39" s="9">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <v>78</v>
+      </c>
+      <c r="G39" s="9">
+        <v>2</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0</v>
+      </c>
+      <c r="I39" s="9">
+        <v>0</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0</v>
+      </c>
+      <c r="K39" s="9">
+        <v>0</v>
+      </c>
+      <c r="L39" s="6">
+        <f t="shared" si="8"/>
+        <v>85</v>
+      </c>
+      <c r="M39" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
         <v>9</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="10">
-        <v>0</v>
-      </c>
-      <c r="M40" s="10">
-        <v>0</v>
+      <c r="B40" s="9">
+        <v>1</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0</v>
+      </c>
+      <c r="D40" s="9">
+        <v>3</v>
+      </c>
+      <c r="E40" s="9">
+        <v>0</v>
+      </c>
+      <c r="F40" s="9">
+        <v>60</v>
+      </c>
+      <c r="G40" s="9">
+        <v>2</v>
+      </c>
+      <c r="H40" s="9">
+        <v>0</v>
+      </c>
+      <c r="I40" s="9">
+        <v>0</v>
+      </c>
+      <c r="J40" s="9">
+        <v>0</v>
+      </c>
+      <c r="K40" s="9">
+        <v>0</v>
+      </c>
+      <c r="L40" s="6">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
+      <c r="M40" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="12">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="10">
         <v>9</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="13">
-        <v>0</v>
-      </c>
-      <c r="M41" s="13">
-        <v>0</v>
+      <c r="B41" s="10">
+        <v>1</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
+        <v>2</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10">
+        <v>110</v>
+      </c>
+      <c r="G41" s="10">
+        <v>2</v>
+      </c>
+      <c r="H41" s="10">
+        <v>0</v>
+      </c>
+      <c r="I41" s="10">
+        <v>0</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0</v>
+      </c>
+      <c r="K41" s="10">
+        <v>0</v>
+      </c>
+      <c r="L41" s="4">
+        <f t="shared" si="8"/>
+        <v>113</v>
+      </c>
+      <c r="M41" s="4">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>10</v>
+      </c>
+      <c r="B42" s="9">
+        <v>4</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0</v>
+      </c>
+      <c r="D42" s="9">
+        <v>5</v>
+      </c>
+      <c r="E42" s="9">
+        <v>0</v>
+      </c>
+      <c r="F42" s="9">
+        <v>0</v>
+      </c>
+      <c r="G42" s="9">
+        <v>0</v>
+      </c>
+      <c r="H42" s="9">
+        <v>1</v>
+      </c>
+      <c r="I42" s="9">
+        <v>2</v>
+      </c>
+      <c r="J42" s="9">
+        <v>4</v>
+      </c>
+      <c r="K42" s="9">
+        <v>0</v>
+      </c>
+      <c r="L42" s="6">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="M42" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="N42" s="11">
+        <f>SUM(L42:L45)</f>
+        <v>424</v>
+      </c>
+      <c r="O42" s="11">
+        <f>SUM(M42:M45)</f>
+        <v>11</v>
+      </c>
+      <c r="P42" s="1">
+        <f>SUM(I42:I45)+SUM(K42:K45)</f>
+        <v>2</v>
+      </c>
+      <c r="Q42" s="1">
+        <f>SUM(C42:C45)+SUM(E42:E45)+SUM(G42:G45)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>10</v>
+      </c>
+      <c r="B43" s="9">
+        <v>4</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0</v>
+      </c>
+      <c r="D43" s="9">
+        <v>2</v>
+      </c>
+      <c r="E43" s="9">
+        <v>0</v>
+      </c>
+      <c r="F43" s="9">
+        <v>55</v>
+      </c>
+      <c r="G43" s="9">
+        <v>1</v>
+      </c>
+      <c r="H43" s="9">
+        <v>0</v>
+      </c>
+      <c r="I43" s="9">
+        <v>0</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0</v>
+      </c>
+      <c r="K43" s="9">
+        <v>0</v>
+      </c>
+      <c r="L43" s="6">
+        <f t="shared" si="8"/>
+        <v>61</v>
+      </c>
+      <c r="M43" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>10</v>
+      </c>
+      <c r="B44" s="9">
+        <v>7</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9">
+        <v>3</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="9">
+        <v>150</v>
+      </c>
+      <c r="G44" s="9">
+        <v>4</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0</v>
+      </c>
+      <c r="I44" s="9">
+        <v>0</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0</v>
+      </c>
+      <c r="K44" s="9">
+        <v>0</v>
+      </c>
+      <c r="L44" s="6">
+        <f t="shared" si="8"/>
+        <v>160</v>
+      </c>
+      <c r="M44" s="6">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="10">
+        <v>10</v>
+      </c>
+      <c r="B45" s="10">
+        <v>8</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10">
+        <v>1</v>
+      </c>
+      <c r="E45" s="10">
+        <v>0</v>
+      </c>
+      <c r="F45" s="10">
+        <v>180</v>
+      </c>
+      <c r="G45" s="10">
+        <v>4</v>
+      </c>
+      <c r="H45" s="10">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10">
+        <v>0</v>
+      </c>
+      <c r="J45" s="10">
+        <v>0</v>
+      </c>
+      <c r="K45" s="10">
+        <v>0</v>
+      </c>
+      <c r="L45" s="4">
+        <f t="shared" si="8"/>
+        <v>189</v>
+      </c>
+      <c r="M45" s="4">
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="P2 P6 P10" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>